<commit_message>
Update phase 2 tasks
</commit_message>
<xml_diff>
--- a/Lab2.Tasks.xlsx
+++ b/Lab2.Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Phase 2 Tasks" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="62">
   <si>
     <t>Get to know your team members. Send them your email, or meet them in class or even outside of class</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -713,9 +716,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,12 +954,16 @@
       <c r="B11" s="23">
         <v>10</v>
       </c>
-      <c r="C11" s="31"/>
+      <c r="C11" s="31" t="s">
+        <v>61</v>
+      </c>
       <c r="D11" s="25"/>
       <c r="E11" s="23"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
-      <c r="H11" s="24"/>
+      <c r="H11" s="24" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
@@ -1004,7 +1011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update task list with correct C file names
</commit_message>
<xml_diff>
--- a/Lab2.Tasks.xlsx
+++ b/Lab2.Tasks.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="64">
   <si>
     <t>Get to know your team members. Send them your email, or meet them in class or even outside of class</t>
   </si>
@@ -147,9 +147,6 @@
     <t>solution-document.docx</t>
   </si>
   <si>
-    <t>int main(argv)</t>
-  </si>
-  <si>
     <t>void init_lister(char)</t>
   </si>
   <si>
@@ -168,15 +165,6 @@
     <t>Phase 2 check list</t>
   </si>
   <si>
-    <t>otherfunct.c</t>
-  </si>
-  <si>
-    <t>printfunct.c</t>
-  </si>
-  <si>
-    <t>utilheader.h</t>
-  </si>
-  <si>
     <t>Phase 1 Task Description</t>
   </si>
   <si>
@@ -186,12 +174,6 @@
     <t>no coding here.  Just header file.</t>
   </si>
   <si>
-    <t>the source was named "util.c" before but I think it should be "lister.c"</t>
-  </si>
-  <si>
-    <t>lister.c</t>
-  </si>
-  <si>
     <t>% Completed</t>
   </si>
   <si>
@@ -208,6 +190,30 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>main.c</t>
+  </si>
+  <si>
+    <t>BOOLEAN get_source_line(FILE *src_file, char src_name[], char todays_date[])</t>
+  </si>
+  <si>
+    <t>FILE *init_lister(const char *name, char source_file_name[], char dte[])</t>
+  </si>
+  <si>
+    <t>int main (int argc, const char *argv[])</t>
+  </si>
+  <si>
+    <t>common.h</t>
+  </si>
+  <si>
+    <t>void print_line(char line[], char source_name_to_print[], char date_to_print[])</t>
+  </si>
+  <si>
+    <t>static void print_page_header(char source_name[], char date[])</t>
+  </si>
+  <si>
+    <t>print.c</t>
   </si>
 </sst>
 </file>
@@ -718,19 +724,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="29" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="29" customWidth="1"/>
-    <col min="8" max="8" width="40.28515625" customWidth="1"/>
+    <col min="4" max="4" width="71.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -739,43 +745,41 @@
         <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="26" t="s">
         <v>52</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>58</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="27"/>
       <c r="G2" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="23"/>
@@ -783,15 +787,15 @@
         <v>2</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="E3" s="23"/>
       <c r="F3" s="28"/>
       <c r="G3" s="28" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H3" s="24"/>
     </row>
@@ -801,19 +805,19 @@
         <v>3</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="27">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H4" s="3"/>
     </row>
@@ -823,15 +827,15 @@
         <v>4</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="28"/>
       <c r="G5" s="28" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H5" s="24"/>
     </row>
@@ -841,15 +845,15 @@
         <v>5</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="27"/>
       <c r="G6" s="27" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H6" s="3"/>
     </row>
@@ -859,10 +863,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="23" t="s">
         <v>18</v>
@@ -871,10 +875,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -883,10 +887,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>18</v>
@@ -895,10 +899,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -907,10 +911,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>18</v>
@@ -919,10 +923,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -931,10 +935,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>18</v>
@@ -943,10 +947,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -955,14 +959,14 @@
         <v>10</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="23"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="24" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1012,7 +1016,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1029,7 +1033,7 @@
         <v>23</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1141,7 +1145,7 @@
         <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Release implementations for main, init_lister and get_source_line functions
</commit_message>
<xml_diff>
--- a/Lab2.Tasks.xlsx
+++ b/Lab2.Tasks.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="65">
   <si>
     <t>Get to know your team members. Send them your email, or meet them in class or even outside of class</t>
   </si>
@@ -189,9 +189,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>main.c</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t>??</t>
+  </si>
+  <si>
+    <t>Yes (0%)</t>
   </si>
 </sst>
 </file>
@@ -723,11 +723,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,7 +738,7 @@
     <col min="4" max="4" width="71.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="29" customWidth="1"/>
     <col min="8" max="8" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -772,19 +772,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F2" s="27">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="H2" s="3"/>
     </row>
@@ -794,10 +794,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>21</v>
@@ -816,19 +816,19 @@
         <v>3</v>
       </c>
       <c r="C4" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="27">
-        <v>0.55000000000000004</v>
+        <v>1</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="H4" s="3"/>
     </row>
@@ -838,13 +838,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="23" t="s">
         <v>63</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>64</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28" t="s">
@@ -858,13 +858,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="27" t="s">
@@ -878,7 +878,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>41</v>
@@ -902,7 +902,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>42</v>
@@ -926,7 +926,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" s="25" t="s">
         <v>43</v>
@@ -950,7 +950,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>44</v>
@@ -967,58 +967,6 @@
       <c r="H10" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23">
-        <v>10</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4">
-        <v>11</v>
-      </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23">
-        <v>12</v>
-      </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="24"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4">
-        <v>13</v>
-      </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>